<commit_message>
added to session list excel sheet
</commit_message>
<xml_diff>
--- a/matlabCode/operantMatching/goodBehDays.xlsx
+++ b/matlabCode/operantMatching/goodBehDays.xlsx
@@ -1,45 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cooper_PC\Desktop\githubRepositories\cooperAnalysis\matlabCode\operantMatching\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{535C5E87-CC6C-4357-A781-678F11E6E888}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC37CD1-9783-45F0-95A5-82CC84FAE76F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21975" windowHeight="16680" tabRatio="875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21975" windowHeight="16680" tabRatio="875" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="29" r:id="rId1"/>
-    <sheet name="CG52" sheetId="47" r:id="rId2"/>
-    <sheet name="CG51" sheetId="46" r:id="rId3"/>
-    <sheet name="dreadds" sheetId="35" r:id="rId4"/>
-    <sheet name="CG50" sheetId="45" r:id="rId5"/>
-    <sheet name="CG49" sheetId="44" r:id="rId6"/>
-    <sheet name="CG48" sheetId="43" r:id="rId7"/>
-    <sheet name="CG47" sheetId="42" r:id="rId8"/>
-    <sheet name="CG46" sheetId="41" r:id="rId9"/>
-    <sheet name="CG45" sheetId="40" r:id="rId10"/>
-    <sheet name="CG44" sheetId="34" r:id="rId11"/>
-    <sheet name="CG43" sheetId="33" r:id="rId12"/>
-    <sheet name="CG42" sheetId="32" r:id="rId13"/>
-    <sheet name="CG41" sheetId="31" r:id="rId14"/>
-    <sheet name="CG25" sheetId="28" r:id="rId15"/>
-    <sheet name="CG24" sheetId="27" r:id="rId16"/>
-    <sheet name="CG23" sheetId="26" r:id="rId17"/>
-    <sheet name="CG18" sheetId="37" r:id="rId18"/>
-    <sheet name="CG16" sheetId="30" r:id="rId19"/>
-    <sheet name="dta" sheetId="36" r:id="rId20"/>
-    <sheet name="CG15" sheetId="11" r:id="rId21"/>
-    <sheet name="CG14" sheetId="9" r:id="rId22"/>
-    <sheet name="CG13" sheetId="3" r:id="rId23"/>
-    <sheet name="CG09" sheetId="2" r:id="rId24"/>
-    <sheet name="CG05" sheetId="10" r:id="rId25"/>
-    <sheet name="CG04" sheetId="25" r:id="rId26"/>
-    <sheet name="CG03" sheetId="24" r:id="rId27"/>
+    <sheet name="CG62" sheetId="51" r:id="rId2"/>
+    <sheet name="CG61" sheetId="50" r:id="rId3"/>
+    <sheet name="CG60" sheetId="49" r:id="rId4"/>
+    <sheet name="CG59" sheetId="48" r:id="rId5"/>
+    <sheet name="CG52" sheetId="47" r:id="rId6"/>
+    <sheet name="CG51" sheetId="46" r:id="rId7"/>
+    <sheet name="dreadds" sheetId="35" r:id="rId8"/>
+    <sheet name="CG50" sheetId="45" r:id="rId9"/>
+    <sheet name="CG49" sheetId="44" r:id="rId10"/>
+    <sheet name="CG48" sheetId="43" r:id="rId11"/>
+    <sheet name="CG47" sheetId="42" r:id="rId12"/>
+    <sheet name="CG46" sheetId="41" r:id="rId13"/>
+    <sheet name="CG45" sheetId="40" r:id="rId14"/>
+    <sheet name="CG44" sheetId="34" r:id="rId15"/>
+    <sheet name="CG43" sheetId="33" r:id="rId16"/>
+    <sheet name="CG42" sheetId="32" r:id="rId17"/>
+    <sheet name="CG41" sheetId="31" r:id="rId18"/>
+    <sheet name="CG25" sheetId="28" r:id="rId19"/>
+    <sheet name="CG24" sheetId="27" r:id="rId20"/>
+    <sheet name="CG23" sheetId="26" r:id="rId21"/>
+    <sheet name="CG18" sheetId="37" r:id="rId22"/>
+    <sheet name="CG16" sheetId="30" r:id="rId23"/>
+    <sheet name="dta" sheetId="36" r:id="rId24"/>
+    <sheet name="CG15" sheetId="11" r:id="rId25"/>
+    <sheet name="CG14" sheetId="9" r:id="rId26"/>
+    <sheet name="CG13" sheetId="3" r:id="rId27"/>
+    <sheet name="CG09" sheetId="2" r:id="rId28"/>
+    <sheet name="CG05" sheetId="10" r:id="rId29"/>
+    <sheet name="CG04" sheetId="25" r:id="rId30"/>
+    <sheet name="CG03" sheetId="24" r:id="rId31"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -54,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2566" uniqueCount="757">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2608" uniqueCount="795">
   <si>
     <t>mCG05d20161115</t>
   </si>
@@ -2325,6 +2329,120 @@
   </si>
   <si>
     <t>mCG52d20180830</t>
+  </si>
+  <si>
+    <t>mCG59d20180914</t>
+  </si>
+  <si>
+    <t>mCG59d20180919</t>
+  </si>
+  <si>
+    <t>mCG59d20180920</t>
+  </si>
+  <si>
+    <t>mCG59d20180921</t>
+  </si>
+  <si>
+    <t>mCG59d20180924</t>
+  </si>
+  <si>
+    <t>mCG59d20180925</t>
+  </si>
+  <si>
+    <t>mCG59d20180926</t>
+  </si>
+  <si>
+    <t>mCG59d20180927</t>
+  </si>
+  <si>
+    <t>mCG59d20181002</t>
+  </si>
+  <si>
+    <t>mCG60d20180914</t>
+  </si>
+  <si>
+    <t>mCG60d20180919</t>
+  </si>
+  <si>
+    <t>mCG60d20180920</t>
+  </si>
+  <si>
+    <t>mCG60d20180921</t>
+  </si>
+  <si>
+    <t>mCG60d20180924</t>
+  </si>
+  <si>
+    <t>mCG60d20180925</t>
+  </si>
+  <si>
+    <t>mCG60d20180926</t>
+  </si>
+  <si>
+    <t>mCG60d20180927</t>
+  </si>
+  <si>
+    <t>mCG60d20181002</t>
+  </si>
+  <si>
+    <t>mCG61d20180914</t>
+  </si>
+  <si>
+    <t>mCG61d20180919</t>
+  </si>
+  <si>
+    <t>mCG61d20180920</t>
+  </si>
+  <si>
+    <t>mCG61d20180921</t>
+  </si>
+  <si>
+    <t>mCG61d20180924</t>
+  </si>
+  <si>
+    <t>mCG61d20180925</t>
+  </si>
+  <si>
+    <t>mCG61d20180926</t>
+  </si>
+  <si>
+    <t>mCG61d20180927</t>
+  </si>
+  <si>
+    <t>mCG61d20181002</t>
+  </si>
+  <si>
+    <t>mCG61d20180913</t>
+  </si>
+  <si>
+    <t>mCG62d20180913</t>
+  </si>
+  <si>
+    <t>mCG62d20180919</t>
+  </si>
+  <si>
+    <t>mCG62d20180920</t>
+  </si>
+  <si>
+    <t>mCG62d20180921</t>
+  </si>
+  <si>
+    <t>mCG62d20180924</t>
+  </si>
+  <si>
+    <t>mCG62d20180925</t>
+  </si>
+  <si>
+    <t>mCG62d20180926</t>
+  </si>
+  <si>
+    <t>mCG62d20181002</t>
+  </si>
+  <si>
+    <t>mCG62d20180916</t>
+  </si>
+  <si>
+    <t>mCG62d20180928</t>
   </si>
 </sst>
 </file>
@@ -4155,6 +4273,895 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76D3787-F720-43BE-BE23-DA7A970762D1}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C1" t="s">
+        <v>550</v>
+      </c>
+      <c r="D1" t="s">
+        <v>553</v>
+      </c>
+      <c r="E1" t="s">
+        <v>717</v>
+      </c>
+      <c r="F1" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>633</v>
+      </c>
+      <c r="B2" t="s">
+        <v>633</v>
+      </c>
+      <c r="C2" t="s">
+        <v>661</v>
+      </c>
+      <c r="D2" t="s">
+        <v>667</v>
+      </c>
+      <c r="E2" t="s">
+        <v>727</v>
+      </c>
+      <c r="F2" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>634</v>
+      </c>
+      <c r="B3" t="s">
+        <v>634</v>
+      </c>
+      <c r="C3" t="s">
+        <v>685</v>
+      </c>
+      <c r="D3" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>635</v>
+      </c>
+      <c r="B4" t="s">
+        <v>635</v>
+      </c>
+      <c r="D4" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>636</v>
+      </c>
+      <c r="B5" t="s">
+        <v>636</v>
+      </c>
+      <c r="D5" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>637</v>
+      </c>
+      <c r="B6" t="s">
+        <v>637</v>
+      </c>
+      <c r="D6" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>638</v>
+      </c>
+      <c r="B7" t="s">
+        <v>638</v>
+      </c>
+      <c r="D7" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>639</v>
+      </c>
+      <c r="B8" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>640</v>
+      </c>
+      <c r="B9" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>641</v>
+      </c>
+      <c r="B10" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>642</v>
+      </c>
+      <c r="B11" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>643</v>
+      </c>
+      <c r="B12" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>661</v>
+      </c>
+      <c r="B13" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>667</v>
+      </c>
+      <c r="B14" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>686</v>
+      </c>
+      <c r="B15" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>728</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CABB42-D828-4499-87B6-7F3ADC11FB6C}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C1" t="s">
+        <v>550</v>
+      </c>
+      <c r="D1" t="s">
+        <v>553</v>
+      </c>
+      <c r="E1" t="s">
+        <v>717</v>
+      </c>
+      <c r="F1" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>622</v>
+      </c>
+      <c r="B2" t="s">
+        <v>622</v>
+      </c>
+      <c r="C2" t="s">
+        <v>660</v>
+      </c>
+      <c r="D2" t="s">
+        <v>666</v>
+      </c>
+      <c r="E2" t="s">
+        <v>725</v>
+      </c>
+      <c r="F2" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>623</v>
+      </c>
+      <c r="B3" t="s">
+        <v>623</v>
+      </c>
+      <c r="C3" t="s">
+        <v>693</v>
+      </c>
+      <c r="D3" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>624</v>
+      </c>
+      <c r="B4" t="s">
+        <v>624</v>
+      </c>
+      <c r="D4" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>625</v>
+      </c>
+      <c r="B5" t="s">
+        <v>625</v>
+      </c>
+      <c r="D5" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>626</v>
+      </c>
+      <c r="B6" t="s">
+        <v>626</v>
+      </c>
+      <c r="D6" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>627</v>
+      </c>
+      <c r="B7" t="s">
+        <v>627</v>
+      </c>
+      <c r="D7" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>628</v>
+      </c>
+      <c r="B8" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>629</v>
+      </c>
+      <c r="B9" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>630</v>
+      </c>
+      <c r="B10" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>631</v>
+      </c>
+      <c r="B11" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>632</v>
+      </c>
+      <c r="B12" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>660</v>
+      </c>
+      <c r="B13" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>666</v>
+      </c>
+      <c r="B14" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>694</v>
+      </c>
+      <c r="B15" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>726</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554766CB-119F-447C-8126-9E9B57290F56}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C1" t="s">
+        <v>550</v>
+      </c>
+      <c r="D1" t="s">
+        <v>553</v>
+      </c>
+      <c r="E1" t="s">
+        <v>717</v>
+      </c>
+      <c r="F1" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>611</v>
+      </c>
+      <c r="B2" t="s">
+        <v>611</v>
+      </c>
+      <c r="C2" t="s">
+        <v>659</v>
+      </c>
+      <c r="D2" t="s">
+        <v>665</v>
+      </c>
+      <c r="E2" t="s">
+        <v>723</v>
+      </c>
+      <c r="F2" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>612</v>
+      </c>
+      <c r="B3" t="s">
+        <v>612</v>
+      </c>
+      <c r="C3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D3" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>613</v>
+      </c>
+      <c r="B4" t="s">
+        <v>613</v>
+      </c>
+      <c r="D4" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>614</v>
+      </c>
+      <c r="B5" t="s">
+        <v>614</v>
+      </c>
+      <c r="D5" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>615</v>
+      </c>
+      <c r="B6" t="s">
+        <v>615</v>
+      </c>
+      <c r="D6" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>616</v>
+      </c>
+      <c r="B7" t="s">
+        <v>616</v>
+      </c>
+      <c r="D7" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>617</v>
+      </c>
+      <c r="B8" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>618</v>
+      </c>
+      <c r="B9" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>619</v>
+      </c>
+      <c r="B10" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>620</v>
+      </c>
+      <c r="B11" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>621</v>
+      </c>
+      <c r="B12" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>659</v>
+      </c>
+      <c r="B13" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>665</v>
+      </c>
+      <c r="B14" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>702</v>
+      </c>
+      <c r="B15" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>724</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4148BF86-A084-4BDF-9BA6-491EC7006D91}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C1" t="s">
+        <v>550</v>
+      </c>
+      <c r="D1" t="s">
+        <v>553</v>
+      </c>
+      <c r="E1" t="s">
+        <v>717</v>
+      </c>
+      <c r="F1" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>600</v>
+      </c>
+      <c r="B2" t="s">
+        <v>600</v>
+      </c>
+      <c r="C2" t="s">
+        <v>658</v>
+      </c>
+      <c r="D2" t="s">
+        <v>664</v>
+      </c>
+      <c r="E2" t="s">
+        <v>721</v>
+      </c>
+      <c r="F2" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>601</v>
+      </c>
+      <c r="B3" t="s">
+        <v>601</v>
+      </c>
+      <c r="C3" t="s">
+        <v>709</v>
+      </c>
+      <c r="D3" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>602</v>
+      </c>
+      <c r="B4" t="s">
+        <v>602</v>
+      </c>
+      <c r="D4" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>603</v>
+      </c>
+      <c r="B5" t="s">
+        <v>603</v>
+      </c>
+      <c r="D5" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>604</v>
+      </c>
+      <c r="B6" t="s">
+        <v>604</v>
+      </c>
+      <c r="D6" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>605</v>
+      </c>
+      <c r="B7" t="s">
+        <v>605</v>
+      </c>
+      <c r="D7" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>606</v>
+      </c>
+      <c r="B8" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>607</v>
+      </c>
+      <c r="B9" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>608</v>
+      </c>
+      <c r="B10" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>609</v>
+      </c>
+      <c r="B11" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>610</v>
+      </c>
+      <c r="B12" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>658</v>
+      </c>
+      <c r="B13" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>664</v>
+      </c>
+      <c r="B14" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>710</v>
+      </c>
+      <c r="B15" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>722</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6F781B-05F7-4138-ADC4-D0EA838F2883}">
   <dimension ref="A1:F24"/>
   <sheetViews>
@@ -4377,7 +5384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F286BCE7-D2D4-4B9A-AF31-2ACEE9F66CC6}">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -4551,7 +5558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323713F2-6459-44D0-B874-19277B3A69D0}">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -4728,7 +5735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96397BA9-EEA8-4258-9642-8C7688374814}">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -4905,7 +5912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B473570-6873-44E7-90C6-6E27741765D2}">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -5083,7 +6090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
@@ -5471,7 +6478,82 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D65198-CD7E-4CD7-8CD5-CC786702D4DF}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>792</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
@@ -5802,7 +6884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
@@ -6158,7 +7240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF34AAB7-AA72-4136-9543-E636C6C2E5C8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -6256,7 +7338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A365224-DE23-4A0D-AA9B-41E155A09F1A}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -6356,94 +7438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{720C92FB-A525-47A2-A0F3-A8556FF1D8E9}">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B1" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>756</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674D1323-1CC6-47F6-80BC-8F163F8DE94C}">
   <dimension ref="A1:B43"/>
   <sheetViews>
@@ -6806,7 +7801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H75"/>
   <sheetViews>
@@ -7821,7 +8816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H70"/>
   <sheetViews>
@@ -8697,7 +9692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
@@ -9070,7 +10065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
@@ -9464,7 +10459,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H87"/>
   <sheetViews>
@@ -10586,7 +11581,82 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8164CABE-2713-4497-BBEB-99AE364EDCD5}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>783</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -10815,7 +11885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
@@ -11144,7 +12214,233 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A43753-457F-4644-84F7-9AEB6B6419BB}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>774</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828A872D-FE31-4D47-9836-89C8B2C030F1}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="3" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>765</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{720C92FB-A525-47A2-A0F3-A8556FF1D8E9}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>756</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69728C59-D8D5-4029-9D54-AAD3E34AA135}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -11231,7 +12527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38DD776-C4BC-4F60-841E-9B220EB8C8EB}">
   <dimension ref="A1:G130"/>
   <sheetViews>
@@ -12374,7 +13670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0AC20A-800D-4328-B206-BB66F7B62008}">
   <dimension ref="A1:F24"/>
   <sheetViews>
@@ -12594,893 +13890,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76D3787-F720-43BE-BE23-DA7A970762D1}">
-  <dimension ref="A1:F24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B1" t="s">
-        <v>549</v>
-      </c>
-      <c r="C1" t="s">
-        <v>550</v>
-      </c>
-      <c r="D1" t="s">
-        <v>553</v>
-      </c>
-      <c r="E1" t="s">
-        <v>717</v>
-      </c>
-      <c r="F1" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>633</v>
-      </c>
-      <c r="B2" t="s">
-        <v>633</v>
-      </c>
-      <c r="C2" t="s">
-        <v>661</v>
-      </c>
-      <c r="D2" t="s">
-        <v>667</v>
-      </c>
-      <c r="E2" t="s">
-        <v>727</v>
-      </c>
-      <c r="F2" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>634</v>
-      </c>
-      <c r="B3" t="s">
-        <v>634</v>
-      </c>
-      <c r="C3" t="s">
-        <v>685</v>
-      </c>
-      <c r="D3" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>635</v>
-      </c>
-      <c r="B4" t="s">
-        <v>635</v>
-      </c>
-      <c r="D4" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>636</v>
-      </c>
-      <c r="B5" t="s">
-        <v>636</v>
-      </c>
-      <c r="D5" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>637</v>
-      </c>
-      <c r="B6" t="s">
-        <v>637</v>
-      </c>
-      <c r="D6" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>638</v>
-      </c>
-      <c r="B7" t="s">
-        <v>638</v>
-      </c>
-      <c r="D7" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>639</v>
-      </c>
-      <c r="B8" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>640</v>
-      </c>
-      <c r="B9" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>641</v>
-      </c>
-      <c r="B10" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>642</v>
-      </c>
-      <c r="B11" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>643</v>
-      </c>
-      <c r="B12" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>661</v>
-      </c>
-      <c r="B13" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>667</v>
-      </c>
-      <c r="B14" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>686</v>
-      </c>
-      <c r="B15" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>728</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CABB42-D828-4499-87B6-7F3ADC11FB6C}">
-  <dimension ref="A1:F24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B1" t="s">
-        <v>549</v>
-      </c>
-      <c r="C1" t="s">
-        <v>550</v>
-      </c>
-      <c r="D1" t="s">
-        <v>553</v>
-      </c>
-      <c r="E1" t="s">
-        <v>717</v>
-      </c>
-      <c r="F1" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>622</v>
-      </c>
-      <c r="B2" t="s">
-        <v>622</v>
-      </c>
-      <c r="C2" t="s">
-        <v>660</v>
-      </c>
-      <c r="D2" t="s">
-        <v>666</v>
-      </c>
-      <c r="E2" t="s">
-        <v>725</v>
-      </c>
-      <c r="F2" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>623</v>
-      </c>
-      <c r="B3" t="s">
-        <v>623</v>
-      </c>
-      <c r="C3" t="s">
-        <v>693</v>
-      </c>
-      <c r="D3" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>624</v>
-      </c>
-      <c r="B4" t="s">
-        <v>624</v>
-      </c>
-      <c r="D4" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>625</v>
-      </c>
-      <c r="B5" t="s">
-        <v>625</v>
-      </c>
-      <c r="D5" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>626</v>
-      </c>
-      <c r="B6" t="s">
-        <v>626</v>
-      </c>
-      <c r="D6" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>627</v>
-      </c>
-      <c r="B7" t="s">
-        <v>627</v>
-      </c>
-      <c r="D7" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>628</v>
-      </c>
-      <c r="B8" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>629</v>
-      </c>
-      <c r="B9" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>630</v>
-      </c>
-      <c r="B10" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>631</v>
-      </c>
-      <c r="B11" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>632</v>
-      </c>
-      <c r="B12" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>660</v>
-      </c>
-      <c r="B13" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>666</v>
-      </c>
-      <c r="B14" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>694</v>
-      </c>
-      <c r="B15" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>726</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554766CB-119F-447C-8126-9E9B57290F56}">
-  <dimension ref="A1:F24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B1" t="s">
-        <v>549</v>
-      </c>
-      <c r="C1" t="s">
-        <v>550</v>
-      </c>
-      <c r="D1" t="s">
-        <v>553</v>
-      </c>
-      <c r="E1" t="s">
-        <v>717</v>
-      </c>
-      <c r="F1" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>611</v>
-      </c>
-      <c r="B2" t="s">
-        <v>611</v>
-      </c>
-      <c r="C2" t="s">
-        <v>659</v>
-      </c>
-      <c r="D2" t="s">
-        <v>665</v>
-      </c>
-      <c r="E2" t="s">
-        <v>723</v>
-      </c>
-      <c r="F2" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>612</v>
-      </c>
-      <c r="B3" t="s">
-        <v>612</v>
-      </c>
-      <c r="C3" t="s">
-        <v>701</v>
-      </c>
-      <c r="D3" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>613</v>
-      </c>
-      <c r="B4" t="s">
-        <v>613</v>
-      </c>
-      <c r="D4" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>614</v>
-      </c>
-      <c r="B5" t="s">
-        <v>614</v>
-      </c>
-      <c r="D5" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>615</v>
-      </c>
-      <c r="B6" t="s">
-        <v>615</v>
-      </c>
-      <c r="D6" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>616</v>
-      </c>
-      <c r="B7" t="s">
-        <v>616</v>
-      </c>
-      <c r="D7" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>617</v>
-      </c>
-      <c r="B8" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>618</v>
-      </c>
-      <c r="B9" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>619</v>
-      </c>
-      <c r="B10" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>620</v>
-      </c>
-      <c r="B11" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>621</v>
-      </c>
-      <c r="B12" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>659</v>
-      </c>
-      <c r="B13" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>665</v>
-      </c>
-      <c r="B14" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>702</v>
-      </c>
-      <c r="B15" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>724</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4148BF86-A084-4BDF-9BA6-491EC7006D91}">
-  <dimension ref="A1:F24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B1" t="s">
-        <v>549</v>
-      </c>
-      <c r="C1" t="s">
-        <v>550</v>
-      </c>
-      <c r="D1" t="s">
-        <v>553</v>
-      </c>
-      <c r="E1" t="s">
-        <v>717</v>
-      </c>
-      <c r="F1" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>600</v>
-      </c>
-      <c r="B2" t="s">
-        <v>600</v>
-      </c>
-      <c r="C2" t="s">
-        <v>658</v>
-      </c>
-      <c r="D2" t="s">
-        <v>664</v>
-      </c>
-      <c r="E2" t="s">
-        <v>721</v>
-      </c>
-      <c r="F2" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>601</v>
-      </c>
-      <c r="B3" t="s">
-        <v>601</v>
-      </c>
-      <c r="C3" t="s">
-        <v>709</v>
-      </c>
-      <c r="D3" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>602</v>
-      </c>
-      <c r="B4" t="s">
-        <v>602</v>
-      </c>
-      <c r="D4" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>603</v>
-      </c>
-      <c r="B5" t="s">
-        <v>603</v>
-      </c>
-      <c r="D5" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>604</v>
-      </c>
-      <c r="B6" t="s">
-        <v>604</v>
-      </c>
-      <c r="D6" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>605</v>
-      </c>
-      <c r="B7" t="s">
-        <v>605</v>
-      </c>
-      <c r="D7" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>606</v>
-      </c>
-      <c r="B8" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>607</v>
-      </c>
-      <c r="B9" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>608</v>
-      </c>
-      <c r="B10" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>609</v>
-      </c>
-      <c r="B11" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>610</v>
-      </c>
-      <c r="B12" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>658</v>
-      </c>
-      <c r="B13" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>664</v>
-      </c>
-      <c r="B14" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>710</v>
-      </c>
-      <c r="B15" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>722</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>